<commit_message>
Save evaluation results: all configs on set A
</commit_message>
<xml_diff>
--- a/Results/set_A/algorithm_results_master_best_setting_200_analysis.xlsx
+++ b/Results/set_A/algorithm_results_master_best_setting_200_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alkraus\ResearchGit\cdrift_adj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alkraus\ResearchGit\cdrift_adj\Results\set_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A6EBB7A-1368-4DDA-AAE1-2B5B722CEE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E772E509-3EF1-4EFD-99F8-FEE209ED93D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696"/>
+    <workbookView xWindow="2838" yWindow="1638" windowWidth="17280" windowHeight="9102" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algorithm_results_master_best_s" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">algorithm_results_master_best_s!$A$1:$D$9</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -85,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -567,9 +580,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -925,11 +939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -952,7 +966,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1">
@@ -963,7 +977,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1">
@@ -974,7 +988,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
@@ -985,7 +999,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1">
@@ -996,7 +1010,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1">
@@ -1007,7 +1021,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="1">
@@ -1018,7 +1032,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="1">
@@ -1029,7 +1043,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1">
@@ -1040,7 +1054,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D9">
+  <autoFilter ref="A1:D9" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
       <sortCondition descending="1" ref="C1:C9"/>
     </sortState>

</xml_diff>